<commit_message>
content setup, theory start, story start
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE94661-CBC6-465E-BC89-0851CD4EC09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E39EFF0-89F4-44DD-A7DD-F38C4C241DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -127,7 +127,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -140,6 +140,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -170,6 +180,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -190,6 +210,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -210,6 +240,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -220,6 +260,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -245,196 +295,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -758,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0396B6C9-CA76-4EFB-9985-7864FF11FF89}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -798,7 +658,7 @@
       </c>
       <c r="F2">
         <f ca="1">_xlfn.DAYS(DATE(2021,10,10),TODAY())</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="1">
         <f>H1+1</f>
@@ -823,10 +683,10 @@
       </c>
       <c r="F3">
         <f ca="1">C11/F2</f>
-        <v>2.3076923076923075</v>
+        <v>2.4</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H36" si="0">H2+1</f>
+        <f t="shared" ref="H3:H5" si="0">H2+1</f>
         <v>44452</v>
       </c>
       <c r="I3">
@@ -838,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -848,7 +708,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>2.2307692307692308</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
@@ -872,6 +732,9 @@
         <f t="shared" si="0"/>
         <v>44454</v>
       </c>
+      <c r="I5">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -884,8 +747,11 @@
         <v>3</v>
       </c>
       <c r="H6" s="1">
-        <f>H5+1</f>
+        <f t="shared" ref="H6:H30" si="1">H5+1</f>
         <v>44455</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -899,8 +765,11 @@
         <v>4</v>
       </c>
       <c r="H7" s="1">
-        <f>H6+1</f>
+        <f t="shared" si="1"/>
         <v>44456</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -914,8 +783,11 @@
         <v>1</v>
       </c>
       <c r="H8" s="1">
-        <f>H7+1</f>
+        <f t="shared" si="1"/>
         <v>44457</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -926,14 +798,20 @@
         <v>10</v>
       </c>
       <c r="H9" s="1">
-        <f>H8+1</f>
+        <f t="shared" si="1"/>
         <v>44458</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H10" s="1">
-        <f>H9+1</f>
+        <f t="shared" si="1"/>
         <v>44459</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -942,15 +820,18 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
         <v>60</v>
       </c>
       <c r="H11" s="1">
-        <f>H10+1</f>
+        <f t="shared" si="1"/>
         <v>44460</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -959,178 +840,226 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>24</v>
+        <v>25.5</v>
       </c>
       <c r="H12" s="1">
-        <f>H11+1</f>
+        <f t="shared" si="1"/>
         <v>44461</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H13" s="1">
-        <f>H12+1</f>
+        <f t="shared" si="1"/>
         <v>44462</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H14" s="1">
-        <f>H13+1</f>
+        <f t="shared" si="1"/>
         <v>44463</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H15" s="1">
-        <f>H14+1</f>
+        <f t="shared" si="1"/>
         <v>44464</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H16" s="1">
-        <f>H15+1</f>
+        <f t="shared" si="1"/>
         <v>44465</v>
       </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H17" s="1">
-        <f>H16+1</f>
+        <f t="shared" si="1"/>
         <v>44466</v>
       </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H18" s="1">
-        <f>H17+1</f>
+        <f t="shared" si="1"/>
         <v>44467</v>
       </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H19" s="1">
-        <f>H18+1</f>
+        <f t="shared" si="1"/>
         <v>44468</v>
       </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H20" s="1">
-        <f>H19+1</f>
+        <f t="shared" si="1"/>
         <v>44469</v>
       </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H21" s="1">
-        <f>H20+1</f>
+        <f t="shared" si="1"/>
         <v>44470</v>
       </c>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H22" s="1">
-        <f>H21+1</f>
+        <f t="shared" si="1"/>
         <v>44471</v>
       </c>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H23" s="1">
-        <f>H22+1</f>
+        <f t="shared" si="1"/>
         <v>44472</v>
       </c>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H24" s="1">
-        <f>H23+1</f>
+        <f t="shared" si="1"/>
         <v>44473</v>
       </c>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H25" s="1">
-        <f>H24+1</f>
+        <f t="shared" si="1"/>
         <v>44474</v>
       </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H26" s="1">
-        <f>H25+1</f>
+        <f t="shared" si="1"/>
         <v>44475</v>
       </c>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H27" s="1">
-        <f>H26+1</f>
+        <f t="shared" si="1"/>
         <v>44476</v>
       </c>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H28" s="1">
-        <f>H27+1</f>
+        <f t="shared" si="1"/>
         <v>44477</v>
       </c>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H29" s="1">
-        <f>H28+1</f>
+        <f t="shared" si="1"/>
         <v>44478</v>
       </c>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.45">
       <c r="H30" s="1">
-        <f>H29+1</f>
+        <f t="shared" si="1"/>
         <v>44479</v>
       </c>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H31" s="1">
-        <f>H30+1</f>
-        <v>44480</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H32" s="1">
-        <f>H31+1</f>
-        <v>44481</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H33" s="1">
-        <f>H32+1</f>
-        <v>44482</v>
-      </c>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H34" s="1">
-        <f>H33+1</f>
-        <v>44483</v>
-      </c>
-    </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H35" s="1">
-        <f>H34+1</f>
-        <v>44484</v>
-      </c>
-    </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="I36">
-        <f>SUM(I1:I35)</f>
-        <v>2</v>
-      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H31" s="1"/>
+      <c r="I31">
+        <f>SUM(I1:I30)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H35" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B11">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
       <formula>$C$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThanOrEqual">
       <formula>$C$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="lessThan">
       <formula>$C$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
       <formula>$F$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>$F$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I30">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>$F$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>$F$4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stories done, game mechanics
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32527D46-1B28-48E7-852E-7B37CEBA3FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3256145-08A5-4698-B5DD-A47695898028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -689,7 +688,7 @@
       </c>
       <c r="F2">
         <f ca="1">_xlfn.DAYS(DATE(2021,10,10),TODAY())</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1">
         <f>H1+1</f>
@@ -714,7 +713,7 @@
       </c>
       <c r="F3">
         <f ca="1">C11/F2</f>
-        <v>3.1578947368421053</v>
+        <v>3.5294117647058822</v>
       </c>
       <c r="H3" s="1">
         <f>H2+1</f>
@@ -729,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -739,7 +738,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>2.8421052631578947</v>
+        <v>2.9411764705882355</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -855,7 +854,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -863,7 +862,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -879,14 +878,14 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>44461</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1055,7 +1054,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
game mechanics done, information
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3256145-08A5-4698-B5DD-A47695898028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AC73C3-D72E-4FFE-A054-FF949D95924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -651,7 +651,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="F2">
         <f ca="1">_xlfn.DAYS(DATE(2021,10,10),TODAY())</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1">
         <f>H1+1</f>
@@ -713,7 +713,7 @@
       </c>
       <c r="F3">
         <f ca="1">C11/F2</f>
-        <v>3.5294117647058822</v>
+        <v>3.75</v>
       </c>
       <c r="H3" s="1">
         <f>H2+1</f>
@@ -728,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -738,7 +738,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>2.9411764705882355</v>
+        <v>2.875</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -854,7 +854,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -862,7 +862,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -878,7 +878,7 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -894,7 +894,7 @@
         <v>44462</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
information almost done - ONLY 2 pages >:(
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AC73C3-D72E-4FFE-A054-FF949D95924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECFA244-14A8-42D2-94BA-3F6F412CE99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -651,7 +651,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -738,7 +738,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>2.875</v>
+        <v>2.75</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -854,7 +854,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -862,7 +862,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -878,7 +878,7 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -903,7 +903,7 @@
         <v>44463</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
information done, multi-agent systems done, consensus almost done
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECFA244-14A8-42D2-94BA-3F6F412CE99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DD5CC2-669D-4C16-B7D9-3BAF07CD7097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -651,7 +651,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="F2">
         <f ca="1">_xlfn.DAYS(DATE(2021,10,10),TODAY())</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1">
         <f>H1+1</f>
@@ -703,6 +703,7 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <f>SUM(I1:I4)</f>
         <v>2</v>
       </c>
       <c r="C3">
@@ -713,7 +714,7 @@
       </c>
       <c r="F3">
         <f ca="1">C11/F2</f>
-        <v>3.75</v>
+        <v>4.2857142857142856</v>
       </c>
       <c r="H3" s="1">
         <f>H2+1</f>
@@ -728,7 +729,8 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <f>SUM(I5:I16)</f>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -738,7 +740,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>2.75</v>
+        <v>2.7142857142857144</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -757,6 +759,7 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <f>SUM(I17:I21)</f>
         <v>0</v>
       </c>
       <c r="C5">
@@ -854,7 +857,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -862,7 +865,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -878,7 +881,7 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -912,7 +915,7 @@
         <v>44464</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1054,7 +1057,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working on Agent, middle of behaviors only 2 pages >:(
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3546C2-9A6C-4650-B78E-E5F5224EB25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C595F8D1-1D25-4D94-B732-1FCFDDFA9BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
       </c>
       <c r="F2">
         <f ca="1">_xlfn.DAYS(DATE(2021,10,10),TODAY())</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1">
         <f>H1+1</f>
@@ -694,7 +694,7 @@
       </c>
       <c r="F3">
         <f ca="1">C11/F2</f>
-        <v>4.615384615384615</v>
+        <v>5.4545454545454541</v>
       </c>
       <c r="H3" s="1">
         <f>H2+1</f>
@@ -720,7 +720,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>2.2307692307692308</v>
+        <v>2.3636363636363638</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -740,7 +740,7 @@
       </c>
       <c r="B5">
         <f>SUM(I17:I21)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>26</v>
@@ -837,7 +837,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -845,7 +845,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -926,7 +926,7 @@
         <v>44467</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="8:9" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
back on track, behaviors, game world, gameplay, dialogue done
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C595F8D1-1D25-4D94-B732-1FCFDDFA9BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9571B295-C736-48A1-95CD-2221707DE2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +720,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>2.3636363636363638</v>
+        <v>1.7727272727272727</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -740,7 +740,7 @@
       </c>
       <c r="B5">
         <f>SUM(I17:I21)</f>
-        <v>8</v>
+        <v>14.5</v>
       </c>
       <c r="C5">
         <v>26</v>
@@ -837,7 +837,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>34</v>
+        <v>40.5</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -845,7 +845,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>26</v>
+        <v>19.5</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>56</v>
+        <v>62.5</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -935,7 +935,7 @@
         <v>44468</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="20" spans="8:9" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>34</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inference, heuristic, quests done
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9571B295-C736-48A1-95CD-2221707DE2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7231A93D-C8C1-4FF7-A1B3-1305F76A6627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
       </c>
       <c r="F2">
         <f ca="1">_xlfn.DAYS(DATE(2021,10,10),TODAY())</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1">
         <f>H1+1</f>
@@ -694,7 +694,7 @@
       </c>
       <c r="F3">
         <f ca="1">C11/F2</f>
-        <v>5.4545454545454541</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1">
         <f>H2+1</f>
@@ -720,7 +720,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>1.7727272727272727</v>
+        <v>1.4</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -740,7 +740,7 @@
       </c>
       <c r="B5">
         <f>SUM(I17:I21)</f>
-        <v>14.5</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>26</v>
@@ -837,7 +837,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>40.5</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -845,7 +845,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>19.5</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>62.5</v>
+        <v>68</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -944,7 +944,7 @@
         <v>44469</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="21" spans="8:9" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>40.5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
implementation one page left
</commit_message>
<xml_diff>
--- a/Thesis/PageCounts.xlsx
+++ b/Thesis/PageCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\Documents\Repositories\Story-generation-with-mutli-agent-systems\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B7D15C-0067-403B-846B-615F40A5FE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A44B3FD-CEFB-4963-928D-9818A9B7CFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{92A426A9-05ED-4761-91B3-DD12145212E5}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -668,7 +668,7 @@
       </c>
       <c r="F2">
         <f ca="1">_xlfn.DAYS(DATE(2021,10,10),TODAY())</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1">
         <f>H1+1</f>
@@ -694,7 +694,7 @@
       </c>
       <c r="F3">
         <f ca="1">C11/F2</f>
-        <v>6.666666666666667</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1">
         <f>H2+1</f>
@@ -720,7 +720,7 @@
       </c>
       <c r="F4">
         <f ca="1">(C11-B11)/F2</f>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="H4" s="3">
         <f>H3+1</f>
@@ -739,11 +739,11 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>SUM(I17:I21)</f>
-        <v>22</v>
+        <f>SUM(I17:I24)</f>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H5" s="1">
         <f>H4+1</f>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ref="H6:H30" si="0">H5+1</f>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="B11">
         <f>SUM(B3:B8)</f>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <f>SUM(C3:C8)</f>
@@ -845,7 +845,7 @@
       </c>
       <c r="D11" s="2">
         <f>C11-B11</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="B12">
         <f>SUM(B2:B9)</f>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -980,7 +980,7 @@
         <v>44473</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="8:9" x14ac:dyDescent="0.45">
@@ -1041,7 +1041,7 @@
       <c r="H31" s="1"/>
       <c r="I31">
         <f>SUM(I1:I30)</f>
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.45">

</xml_diff>